<commit_message>
Ligenhistorie England bis Platz 11
</commit_message>
<xml_diff>
--- a/England/Premier League/Ligenhistorie.xlsx
+++ b/England/Premier League/Ligenhistorie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Desktop\footballstats\footballstats\England\Premier League\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBCDD78-8D61-4944-8722-C0A22A3C1924}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34821250-B6B0-4573-A2AB-31391985CF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1800" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="2490" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
   <si>
     <t>Vereine</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>Sunderland AFC</t>
+  </si>
+  <si>
+    <t>West Bromwich Albion</t>
+  </si>
+  <si>
+    <t>Blackburn Rovers</t>
   </si>
 </sst>
 </file>
@@ -406,7 +412,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -414,11 +420,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -441,6 +462,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -723,22 +747,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DT11"/>
+  <dimension ref="A1:DT13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DD1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="DT10" sqref="DT10"/>
+      <selection pane="bottomLeft" activeCell="AX13" sqref="AX13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="124" width="4.7109375" style="1" customWidth="1"/>
     <col min="125" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1142,7 +1166,7 @@
       <c r="N2" s="8">
         <v>10</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="10">
         <v>1</v>
       </c>
       <c r="P2" s="8">
@@ -1157,7 +1181,7 @@
       <c r="S2" s="7">
         <v>1</v>
       </c>
-      <c r="T2" s="8">
+      <c r="T2" s="10">
         <v>1</v>
       </c>
       <c r="U2" s="8">
@@ -1193,10 +1217,10 @@
       <c r="AE2" s="8">
         <v>4</v>
       </c>
-      <c r="AF2" s="8">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="8">
+      <c r="AF2" s="10">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="10">
         <v>1</v>
       </c>
       <c r="AH2" s="8">
@@ -1247,7 +1271,7 @@
       <c r="AW2" s="8">
         <v>11</v>
       </c>
-      <c r="AX2" s="8">
+      <c r="AX2" s="10">
         <v>1</v>
       </c>
       <c r="AY2" s="8">
@@ -1298,13 +1322,13 @@
       <c r="BN2" s="8">
         <v>8</v>
       </c>
-      <c r="BO2" s="8">
+      <c r="BO2" s="10">
         <v>1</v>
       </c>
       <c r="BP2" s="8">
         <v>7</v>
       </c>
-      <c r="BQ2" s="8">
+      <c r="BQ2" s="10">
         <v>1</v>
       </c>
       <c r="BR2" s="8">
@@ -1325,7 +1349,7 @@
       <c r="BW2" s="8">
         <v>3</v>
       </c>
-      <c r="BX2" s="8">
+      <c r="BX2" s="10">
         <v>1</v>
       </c>
       <c r="BY2" s="8">
@@ -1334,49 +1358,49 @@
       <c r="BZ2" s="8">
         <v>3</v>
       </c>
-      <c r="CA2" s="8">
-        <v>1</v>
-      </c>
-      <c r="CB2" s="8">
+      <c r="CA2" s="10">
+        <v>1</v>
+      </c>
+      <c r="CB2" s="10">
         <v>1</v>
       </c>
       <c r="CC2" s="8">
         <v>2</v>
       </c>
-      <c r="CD2" s="8">
-        <v>1</v>
-      </c>
-      <c r="CE2" s="8">
+      <c r="CD2" s="10">
+        <v>1</v>
+      </c>
+      <c r="CE2" s="10">
         <v>1</v>
       </c>
       <c r="CF2" s="8">
         <v>5</v>
       </c>
-      <c r="CG2" s="8">
-        <v>1</v>
-      </c>
-      <c r="CH2" s="8">
-        <v>1</v>
-      </c>
-      <c r="CI2" s="8">
+      <c r="CG2" s="10">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="10">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="10">
         <v>1</v>
       </c>
       <c r="CJ2" s="8">
         <v>2</v>
       </c>
-      <c r="CK2" s="8">
+      <c r="CK2" s="10">
         <v>1</v>
       </c>
       <c r="CL2" s="8">
         <v>2</v>
       </c>
-      <c r="CM2" s="8">
+      <c r="CM2" s="10">
         <v>1</v>
       </c>
       <c r="CN2" s="8">
         <v>2</v>
       </c>
-      <c r="CO2" s="8">
+      <c r="CO2" s="10">
         <v>1</v>
       </c>
       <c r="CP2" s="8">
@@ -1466,14 +1490,14 @@
       <c r="DR2" s="8">
         <v>2</v>
       </c>
-      <c r="DS2" s="8">
+      <c r="DS2" s="10">
         <v>1</v>
       </c>
       <c r="DT2" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1584,19 +1608,19 @@
       <c r="AN3" s="8">
         <v>14</v>
       </c>
-      <c r="AO3" s="8">
+      <c r="AO3" s="10">
         <v>1</v>
       </c>
       <c r="AP3" s="8">
         <v>2</v>
       </c>
-      <c r="AQ3" s="8">
-        <v>1</v>
-      </c>
-      <c r="AR3" s="8">
-        <v>1</v>
-      </c>
-      <c r="AS3" s="8">
+      <c r="AQ3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AR3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="10">
         <v>1</v>
       </c>
       <c r="AT3" s="8">
@@ -1605,7 +1629,7 @@
       <c r="AU3" s="8">
         <v>3</v>
       </c>
-      <c r="AV3" s="8">
+      <c r="AV3" s="10">
         <v>1</v>
       </c>
       <c r="AW3" s="8">
@@ -1614,7 +1638,7 @@
       <c r="AX3" s="8">
         <v>13</v>
       </c>
-      <c r="AY3" s="8">
+      <c r="AY3" s="10">
         <v>1</v>
       </c>
       <c r="AZ3" s="8">
@@ -1629,7 +1653,7 @@
       <c r="BC3" s="8">
         <v>3</v>
       </c>
-      <c r="BD3" s="8">
+      <c r="BD3" s="10">
         <v>1</v>
       </c>
       <c r="BE3" s="8">
@@ -1683,7 +1707,7 @@
       <c r="BU3" s="8">
         <v>12</v>
       </c>
-      <c r="BV3" s="8">
+      <c r="BV3" s="10">
         <v>1</v>
       </c>
       <c r="BW3" s="8">
@@ -1737,13 +1761,13 @@
       <c r="CM3" s="8">
         <v>6</v>
       </c>
-      <c r="CN3" s="8">
+      <c r="CN3" s="10">
         <v>1</v>
       </c>
       <c r="CO3" s="8">
         <v>4</v>
       </c>
-      <c r="CP3" s="8">
+      <c r="CP3" s="10">
         <v>1</v>
       </c>
       <c r="CQ3" s="8">
@@ -1764,7 +1788,7 @@
       <c r="CV3" s="8">
         <v>3</v>
       </c>
-      <c r="CW3" s="8">
+      <c r="CW3" s="10">
         <v>1</v>
       </c>
       <c r="CX3" s="8">
@@ -1776,13 +1800,13 @@
       <c r="CZ3" s="8">
         <v>2</v>
       </c>
-      <c r="DA3" s="8">
+      <c r="DA3" s="10">
         <v>1</v>
       </c>
       <c r="DB3" s="8">
         <v>2</v>
       </c>
-      <c r="DC3" s="8">
+      <c r="DC3" s="10">
         <v>1</v>
       </c>
       <c r="DD3" s="8">
@@ -1837,7 +1861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1850,7 +1874,7 @@
       <c r="D4" s="8">
         <v>2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="10">
         <v>1</v>
       </c>
       <c r="F4" s="8">
@@ -1922,7 +1946,7 @@
       <c r="AB4" s="8">
         <v>15</v>
       </c>
-      <c r="AC4" s="8">
+      <c r="AC4" s="10">
         <v>1</v>
       </c>
       <c r="AD4" s="8">
@@ -1949,7 +1973,7 @@
       <c r="AK4" s="8">
         <v>20</v>
       </c>
-      <c r="AL4" s="8">
+      <c r="AL4" s="10">
         <v>1</v>
       </c>
       <c r="AM4" s="8">
@@ -1961,7 +1985,7 @@
       <c r="AO4" s="7">
         <v>1</v>
       </c>
-      <c r="AP4" s="8">
+      <c r="AP4" s="10">
         <v>1</v>
       </c>
       <c r="AQ4" s="8">
@@ -1982,7 +2006,7 @@
       <c r="AV4" s="8">
         <v>14</v>
       </c>
-      <c r="AW4" s="8">
+      <c r="AW4" s="10">
         <v>1</v>
       </c>
       <c r="AX4" s="8">
@@ -2033,7 +2057,7 @@
       <c r="BM4" s="8">
         <v>4</v>
       </c>
-      <c r="BN4" s="8">
+      <c r="BN4" s="10">
         <v>1</v>
       </c>
       <c r="BO4" s="8">
@@ -2054,7 +2078,7 @@
       <c r="BT4" s="8">
         <v>3</v>
       </c>
-      <c r="BU4" s="8">
+      <c r="BU4" s="10">
         <v>1</v>
       </c>
       <c r="BV4" s="8">
@@ -2099,13 +2123,13 @@
       <c r="CI4" s="8">
         <v>7</v>
       </c>
-      <c r="CJ4" s="8">
+      <c r="CJ4" s="10">
         <v>1</v>
       </c>
       <c r="CK4" s="8">
         <v>2</v>
       </c>
-      <c r="CL4" s="8">
+      <c r="CL4" s="10">
         <v>1</v>
       </c>
       <c r="CM4" s="8">
@@ -2211,7 +2235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2267,7 +2291,7 @@
       <c r="U5" s="8">
         <v>8</v>
       </c>
-      <c r="V5" s="8">
+      <c r="V5" s="10">
         <v>1</v>
       </c>
       <c r="W5" s="8">
@@ -2276,7 +2300,7 @@
       <c r="X5" s="8">
         <v>5</v>
       </c>
-      <c r="Y5" s="8">
+      <c r="Y5" s="10">
         <v>1</v>
       </c>
       <c r="Z5" s="8">
@@ -2366,7 +2390,7 @@
       <c r="BB5" s="8">
         <v>2</v>
       </c>
-      <c r="BC5" s="8">
+      <c r="BC5" s="10">
         <v>1</v>
       </c>
       <c r="BD5" s="8">
@@ -2378,10 +2402,10 @@
       <c r="BF5" s="8">
         <v>5</v>
       </c>
-      <c r="BG5" s="8">
-        <v>1</v>
-      </c>
-      <c r="BH5" s="8">
+      <c r="BG5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BH5" s="10">
         <v>1</v>
       </c>
       <c r="BI5" s="8">
@@ -2405,13 +2429,13 @@
       <c r="BO5" s="8">
         <v>2</v>
       </c>
-      <c r="BP5" s="8">
+      <c r="BP5" s="10">
         <v>1</v>
       </c>
       <c r="BQ5" s="8">
         <v>4</v>
       </c>
-      <c r="BR5" s="8">
+      <c r="BR5" s="10">
         <v>1</v>
       </c>
       <c r="BS5" s="8">
@@ -2489,37 +2513,37 @@
       <c r="CQ5" s="8">
         <v>2</v>
       </c>
-      <c r="CR5" s="8">
-        <v>1</v>
-      </c>
-      <c r="CS5" s="8">
+      <c r="CR5" s="10">
+        <v>1</v>
+      </c>
+      <c r="CS5" s="10">
         <v>1</v>
       </c>
       <c r="CT5" s="8">
         <v>2</v>
       </c>
-      <c r="CU5" s="8">
-        <v>1</v>
-      </c>
-      <c r="CV5" s="8">
+      <c r="CU5" s="10">
+        <v>1</v>
+      </c>
+      <c r="CV5" s="10">
         <v>1</v>
       </c>
       <c r="CW5" s="8">
         <v>2</v>
       </c>
-      <c r="CX5" s="8">
-        <v>1</v>
-      </c>
-      <c r="CY5" s="8">
-        <v>1</v>
-      </c>
-      <c r="CZ5" s="8">
+      <c r="CX5" s="10">
+        <v>1</v>
+      </c>
+      <c r="CY5" s="10">
+        <v>1</v>
+      </c>
+      <c r="CZ5" s="10">
         <v>1</v>
       </c>
       <c r="DA5" s="8">
         <v>3</v>
       </c>
-      <c r="DB5" s="8">
+      <c r="DB5" s="10">
         <v>1</v>
       </c>
       <c r="DC5" s="8">
@@ -2531,25 +2555,25 @@
       <c r="DE5" s="8">
         <v>2</v>
       </c>
-      <c r="DF5" s="8">
-        <v>1</v>
-      </c>
-      <c r="DG5" s="8">
-        <v>1</v>
-      </c>
-      <c r="DH5" s="8">
+      <c r="DF5" s="10">
+        <v>1</v>
+      </c>
+      <c r="DG5" s="10">
+        <v>1</v>
+      </c>
+      <c r="DH5" s="10">
         <v>1</v>
       </c>
       <c r="DI5" s="8">
         <v>2</v>
       </c>
-      <c r="DJ5" s="8">
+      <c r="DJ5" s="10">
         <v>1</v>
       </c>
       <c r="DK5" s="8">
         <v>2</v>
       </c>
-      <c r="DL5" s="8">
+      <c r="DL5" s="10">
         <v>1</v>
       </c>
       <c r="DM5" s="8">
@@ -2577,7 +2601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2599,25 +2623,25 @@
       <c r="G6" s="8">
         <v>4</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="10">
         <v>1</v>
       </c>
       <c r="I6" s="8">
         <v>3</v>
       </c>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="J6" s="10">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10">
         <v>1</v>
       </c>
       <c r="L6" s="8">
         <v>6</v>
       </c>
-      <c r="M6" s="8">
-        <v>1</v>
-      </c>
-      <c r="N6" s="8">
+      <c r="M6" s="10">
+        <v>1</v>
+      </c>
+      <c r="N6" s="10">
         <v>1</v>
       </c>
       <c r="O6" s="8">
@@ -2647,7 +2671,7 @@
       <c r="W6" s="8">
         <v>7</v>
       </c>
-      <c r="X6" s="8">
+      <c r="X6" s="10">
         <v>1</v>
       </c>
       <c r="Y6" s="8">
@@ -2827,7 +2851,7 @@
       <c r="CE6" s="8">
         <v>7</v>
       </c>
-      <c r="CF6" s="8">
+      <c r="CF6" s="10">
         <v>1</v>
       </c>
       <c r="CG6" s="8">
@@ -2951,7 +2975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3082,7 +3106,7 @@
       <c r="AT7" s="8">
         <v>9</v>
       </c>
-      <c r="AU7" s="8">
+      <c r="AU7" s="10">
         <v>1</v>
       </c>
       <c r="AV7" s="8">
@@ -3154,7 +3178,7 @@
       <c r="BR7" s="8">
         <v>15</v>
       </c>
-      <c r="BS7" s="8">
+      <c r="BS7" s="10">
         <v>1</v>
       </c>
       <c r="BT7" s="8">
@@ -3286,13 +3310,13 @@
       <c r="DJ7" s="8">
         <v>3</v>
       </c>
-      <c r="DK7" s="8">
+      <c r="DK7" s="10">
         <v>1</v>
       </c>
       <c r="DL7" s="8">
         <v>2</v>
       </c>
-      <c r="DM7" s="8">
+      <c r="DM7" s="10">
         <v>1</v>
       </c>
       <c r="DN7" s="8">
@@ -3304,20 +3328,20 @@
       <c r="DP7" s="8">
         <v>3</v>
       </c>
-      <c r="DQ7" s="8">
-        <v>1</v>
-      </c>
-      <c r="DR7" s="8">
+      <c r="DQ7" s="10">
+        <v>1</v>
+      </c>
+      <c r="DR7" s="10">
         <v>1</v>
       </c>
       <c r="DS7" s="8">
         <v>2</v>
       </c>
-      <c r="DT7" s="8">
+      <c r="DT7" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3437,7 +3461,7 @@
       <c r="BA8" s="7">
         <v>1</v>
       </c>
-      <c r="BB8" s="8">
+      <c r="BB8" s="10">
         <v>1</v>
       </c>
       <c r="BC8" s="8">
@@ -3467,7 +3491,7 @@
       <c r="BK8" s="8">
         <v>3</v>
       </c>
-      <c r="BL8" s="8">
+      <c r="BL8" s="10">
         <v>1</v>
       </c>
       <c r="BM8" s="8">
@@ -3651,7 +3675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3789,7 +3813,7 @@
       <c r="BE9" s="8">
         <v>8</v>
       </c>
-      <c r="BF9" s="8">
+      <c r="BF9" s="10">
         <v>1</v>
       </c>
       <c r="BG9" s="8">
@@ -3939,10 +3963,10 @@
       <c r="DC9" s="8">
         <v>2</v>
       </c>
-      <c r="DD9" s="8">
-        <v>1</v>
-      </c>
-      <c r="DE9" s="8">
+      <c r="DD9" s="10">
+        <v>1</v>
+      </c>
+      <c r="DE9" s="10">
         <v>1</v>
       </c>
       <c r="DF9" s="8">
@@ -3954,7 +3978,7 @@
       <c r="DH9" s="8">
         <v>3</v>
       </c>
-      <c r="DI9" s="8">
+      <c r="DI9" s="10">
         <v>1</v>
       </c>
       <c r="DJ9" s="8">
@@ -3969,13 +3993,13 @@
       <c r="DM9" s="8">
         <v>3</v>
       </c>
-      <c r="DN9" s="8">
+      <c r="DN9" s="10">
         <v>1</v>
       </c>
       <c r="DO9" s="8">
         <v>10</v>
       </c>
-      <c r="DP9" s="8">
+      <c r="DP9" s="10">
         <v>1</v>
       </c>
       <c r="DQ9" s="8">
@@ -3991,7 +4015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4036,19 +4060,19 @@
       <c r="R10" s="8">
         <v>4</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10" s="10">
         <v>1</v>
       </c>
       <c r="T10" s="8">
         <v>4</v>
       </c>
-      <c r="U10" s="8">
+      <c r="U10" s="10">
         <v>1</v>
       </c>
       <c r="V10" s="8">
         <v>4</v>
       </c>
-      <c r="W10" s="8">
+      <c r="W10" s="10">
         <v>1</v>
       </c>
       <c r="X10" s="8">
@@ -4090,7 +4114,7 @@
       <c r="AJ10" s="8">
         <v>10</v>
       </c>
-      <c r="AK10" s="8">
+      <c r="AK10" s="10">
         <v>1</v>
       </c>
       <c r="AL10" s="8">
@@ -4355,7 +4379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4367,16 +4391,16 @@
       <c r="E11" s="8">
         <v>7</v>
       </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8">
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10">
         <v>1</v>
       </c>
       <c r="H11" s="8">
         <v>2</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="10">
         <v>1</v>
       </c>
       <c r="J11" s="8">
@@ -4397,7 +4421,7 @@
       <c r="O11" s="8">
         <v>2</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11" s="10">
         <v>1</v>
       </c>
       <c r="Q11" s="8">
@@ -4430,7 +4454,7 @@
       <c r="Z11" s="8">
         <v>8</v>
       </c>
-      <c r="AA11" s="8">
+      <c r="AA11" s="10">
         <v>1</v>
       </c>
       <c r="AB11" s="8">
@@ -4487,7 +4511,7 @@
       <c r="AS11" s="8">
         <v>2</v>
       </c>
-      <c r="AT11" s="8">
+      <c r="AT11" s="10">
         <v>1</v>
       </c>
       <c r="AU11" s="8">
@@ -4723,6 +4747,520 @@
       </c>
       <c r="DT11" s="9">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6</v>
+      </c>
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8">
+        <v>12</v>
+      </c>
+      <c r="F12" s="8">
+        <v>12</v>
+      </c>
+      <c r="G12" s="8">
+        <v>8</v>
+      </c>
+      <c r="H12" s="8">
+        <v>8</v>
+      </c>
+      <c r="I12" s="8">
+        <v>13</v>
+      </c>
+      <c r="J12" s="8">
+        <v>16</v>
+      </c>
+      <c r="K12" s="8">
+        <v>12</v>
+      </c>
+      <c r="L12" s="8">
+        <v>7</v>
+      </c>
+      <c r="M12" s="8">
+        <v>14</v>
+      </c>
+      <c r="N12" s="8">
+        <v>13</v>
+      </c>
+      <c r="O12" s="8">
+        <v>16</v>
+      </c>
+      <c r="P12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>7</v>
+      </c>
+      <c r="R12" s="8">
+        <v>18</v>
+      </c>
+      <c r="S12" s="7">
+        <v>10</v>
+      </c>
+      <c r="T12" s="7">
+        <v>4</v>
+      </c>
+      <c r="U12" s="7">
+        <v>4</v>
+      </c>
+      <c r="V12" s="7">
+        <v>5</v>
+      </c>
+      <c r="W12" s="7">
+        <v>3</v>
+      </c>
+      <c r="X12" s="7">
+        <v>11</v>
+      </c>
+      <c r="Y12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="8">
+        <v>9</v>
+      </c>
+      <c r="AA12" s="8">
+        <v>10</v>
+      </c>
+      <c r="AB12" s="8">
+        <v>5</v>
+      </c>
+      <c r="AC12" s="8">
+        <v>10</v>
+      </c>
+      <c r="AD12" s="10">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="8">
+        <v>14</v>
+      </c>
+      <c r="AF12" s="8">
+        <v>13</v>
+      </c>
+      <c r="AG12" s="8">
+        <v>7</v>
+      </c>
+      <c r="AH12" s="8">
+        <v>16</v>
+      </c>
+      <c r="AI12" s="8">
+        <v>2</v>
+      </c>
+      <c r="AJ12" s="8">
+        <v>13</v>
+      </c>
+      <c r="AK12" s="8">
+        <v>22</v>
+      </c>
+      <c r="AL12" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM12" s="7">
+        <v>7</v>
+      </c>
+      <c r="AN12" s="7">
+        <v>6</v>
+      </c>
+      <c r="AO12" s="7">
+        <v>2</v>
+      </c>
+      <c r="AP12" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ12" s="8">
+        <v>4</v>
+      </c>
+      <c r="AR12" s="8">
+        <v>7</v>
+      </c>
+      <c r="AS12" s="8">
+        <v>9</v>
+      </c>
+      <c r="AT12" s="8">
+        <v>18</v>
+      </c>
+      <c r="AU12" s="8">
+        <v>16</v>
+      </c>
+      <c r="AV12" s="8">
+        <v>22</v>
+      </c>
+      <c r="AW12" s="7">
+        <v>10</v>
+      </c>
+      <c r="AX12" s="7">
+        <v>7</v>
+      </c>
+      <c r="AY12" s="7">
+        <v>7</v>
+      </c>
+      <c r="AZ12" s="7">
+        <v>2</v>
+      </c>
+      <c r="BA12" s="8">
+        <v>14</v>
+      </c>
+      <c r="BB12" s="8">
+        <v>16</v>
+      </c>
+      <c r="BC12" s="8">
+        <v>13</v>
+      </c>
+      <c r="BD12" s="8">
+        <v>4</v>
+      </c>
+      <c r="BE12" s="8">
+        <v>2</v>
+      </c>
+      <c r="BF12" s="8">
+        <v>17</v>
+      </c>
+      <c r="BG12" s="8">
+        <v>13</v>
+      </c>
+      <c r="BH12" s="8">
+        <v>11</v>
+      </c>
+      <c r="BI12" s="8">
+        <v>4</v>
+      </c>
+      <c r="BJ12" s="8">
+        <v>5</v>
+      </c>
+      <c r="BK12" s="8">
+        <v>4</v>
+      </c>
+      <c r="BL12" s="8">
+        <v>10</v>
+      </c>
+      <c r="BM12" s="8">
+        <v>9</v>
+      </c>
+      <c r="BN12" s="8">
+        <v>14</v>
+      </c>
+      <c r="BO12" s="8">
+        <v>10</v>
+      </c>
+      <c r="BP12" s="8">
+        <v>14</v>
+      </c>
+      <c r="BQ12" s="8">
+        <v>6</v>
+      </c>
+      <c r="BR12" s="8">
+        <v>13</v>
+      </c>
+      <c r="BS12" s="8">
+        <v>8</v>
+      </c>
+      <c r="BT12" s="8">
+        <v>10</v>
+      </c>
+      <c r="BU12" s="8">
+        <v>16</v>
+      </c>
+      <c r="BV12" s="8">
+        <v>17</v>
+      </c>
+      <c r="BW12" s="8">
+        <v>16</v>
+      </c>
+      <c r="BX12" s="8">
+        <v>22</v>
+      </c>
+      <c r="BY12" s="7">
+        <v>8</v>
+      </c>
+      <c r="BZ12" s="7">
+        <v>6</v>
+      </c>
+      <c r="CA12" s="7">
+        <v>3</v>
+      </c>
+      <c r="CB12" s="8">
+        <v>7</v>
+      </c>
+      <c r="CC12" s="8">
+        <v>6</v>
+      </c>
+      <c r="CD12" s="8">
+        <v>3</v>
+      </c>
+      <c r="CE12" s="8">
+        <v>10</v>
+      </c>
+      <c r="CF12" s="8">
+        <v>4</v>
+      </c>
+      <c r="CG12" s="8">
+        <v>17</v>
+      </c>
+      <c r="CH12" s="8">
+        <v>11</v>
+      </c>
+      <c r="CI12" s="8">
+        <v>17</v>
+      </c>
+      <c r="CJ12" s="8">
+        <v>12</v>
+      </c>
+      <c r="CK12" s="8">
+        <v>22</v>
+      </c>
+      <c r="CL12" s="7">
+        <v>15</v>
+      </c>
+      <c r="CM12" s="7">
+        <v>20</v>
+      </c>
+      <c r="CN12" s="7">
+        <v>9</v>
+      </c>
+      <c r="CO12" s="7">
+        <v>20</v>
+      </c>
+      <c r="CP12" s="7">
+        <v>23</v>
+      </c>
+      <c r="CQ12" s="9">
+        <v>7</v>
+      </c>
+      <c r="CR12" s="9">
+        <v>4</v>
+      </c>
+      <c r="CS12" s="7">
+        <v>21</v>
+      </c>
+      <c r="CT12" s="7">
+        <v>19</v>
+      </c>
+      <c r="CU12" s="7">
+        <v>11</v>
+      </c>
+      <c r="CV12" s="7">
+        <v>16</v>
+      </c>
+      <c r="CW12" s="7">
+        <v>10</v>
+      </c>
+      <c r="CX12" s="7">
+        <v>12</v>
+      </c>
+      <c r="CY12" s="7">
+        <v>21</v>
+      </c>
+      <c r="CZ12" s="7">
+        <v>6</v>
+      </c>
+      <c r="DA12" s="7">
+        <v>2</v>
+      </c>
+      <c r="DB12" s="8">
+        <v>19</v>
+      </c>
+      <c r="DC12" s="7">
+        <v>2</v>
+      </c>
+      <c r="DD12" s="8">
+        <v>17</v>
+      </c>
+      <c r="DE12" s="8">
+        <v>19</v>
+      </c>
+      <c r="DF12" s="7">
+        <v>4</v>
+      </c>
+      <c r="DG12" s="7">
+        <v>1</v>
+      </c>
+      <c r="DH12" s="8">
+        <v>20</v>
+      </c>
+      <c r="DI12" s="7">
+        <v>2</v>
+      </c>
+      <c r="DJ12" s="8">
+        <v>11</v>
+      </c>
+      <c r="DK12" s="8">
+        <v>10</v>
+      </c>
+      <c r="DL12" s="8">
+        <v>8</v>
+      </c>
+      <c r="DM12" s="8">
+        <v>17</v>
+      </c>
+      <c r="DN12" s="8">
+        <v>13</v>
+      </c>
+      <c r="DO12" s="8">
+        <v>14</v>
+      </c>
+      <c r="DP12" s="8">
+        <v>10</v>
+      </c>
+      <c r="DQ12" s="8">
+        <v>20</v>
+      </c>
+      <c r="DR12" s="7">
+        <v>4</v>
+      </c>
+      <c r="DS12" s="7">
+        <v>2</v>
+      </c>
+      <c r="DT12" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:124" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>6</v>
+      </c>
+      <c r="F13" s="8">
+        <v>9</v>
+      </c>
+      <c r="G13" s="8">
+        <v>9</v>
+      </c>
+      <c r="H13" s="8">
+        <v>4</v>
+      </c>
+      <c r="I13" s="8">
+        <v>5</v>
+      </c>
+      <c r="J13" s="8">
+        <v>8</v>
+      </c>
+      <c r="K13" s="8">
+        <v>14</v>
+      </c>
+      <c r="L13" s="8">
+        <v>15</v>
+      </c>
+      <c r="M13" s="8">
+        <v>6</v>
+      </c>
+      <c r="N13" s="8">
+        <v>14</v>
+      </c>
+      <c r="O13" s="8">
+        <v>9</v>
+      </c>
+      <c r="P13" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>16</v>
+      </c>
+      <c r="R13" s="8">
+        <v>15</v>
+      </c>
+      <c r="S13" s="8">
+        <v>13</v>
+      </c>
+      <c r="T13" s="8">
+        <v>9</v>
+      </c>
+      <c r="U13" s="8">
+        <v>12</v>
+      </c>
+      <c r="V13" s="8">
+        <v>14</v>
+      </c>
+      <c r="W13" s="8">
+        <v>4</v>
+      </c>
+      <c r="X13" s="8">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>12</v>
+      </c>
+      <c r="Z13" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>5</v>
+      </c>
+      <c r="AB13" s="10">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="8">
+        <v>20</v>
+      </c>
+      <c r="AE13" s="8">
+        <v>11</v>
+      </c>
+      <c r="AF13" s="8">
+        <v>15</v>
+      </c>
+      <c r="AG13" s="8">
+        <v>14</v>
+      </c>
+      <c r="AH13" s="8">
+        <v>8</v>
+      </c>
+      <c r="AI13" s="8">
+        <v>16</v>
+      </c>
+      <c r="AJ13" s="8">
+        <v>12</v>
+      </c>
+      <c r="AK13" s="8">
+        <v>18</v>
+      </c>
+      <c r="AL13" s="8">
+        <v>12</v>
+      </c>
+      <c r="AM13" s="8">
+        <v>7</v>
+      </c>
+      <c r="AN13" s="8">
+        <v>6</v>
+      </c>
+      <c r="AO13" s="8">
+        <v>10</v>
+      </c>
+      <c r="AP13" s="8">
+        <v>16</v>
+      </c>
+      <c r="AQ13" s="8">
+        <v>15</v>
+      </c>
+      <c r="AR13" s="8">
+        <v>8</v>
+      </c>
+      <c r="AS13" s="8">
+        <v>15</v>
+      </c>
+      <c r="AT13" s="8">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>